<commit_message>
add Modules & HMI (.mer)
</commit_message>
<xml_diff>
--- a/TagListHmi.xlsx
+++ b/TagListHmi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\J1405-Haynes-SavageSaw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A613D506-0D2A-4ECB-85A1-A61E909C547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0C94EB-DFAF-4380-9B02-490094C8E109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6A31735C-1E10-47DA-9BDD-C0801E160811}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6A31735C-1E10-47DA-9BDD-C0801E160811}"/>
   </bookViews>
   <sheets>
     <sheet name="TagListHmi" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="932">
   <si>
     <t>// Name</t>
   </si>
@@ -2804,6 +2804,21 @@
   </si>
   <si>
     <t>Motion to PLC</t>
+  </si>
+  <si>
+    <t>Note:  Indicators for:</t>
+  </si>
+  <si>
+    <t>Auto Gauge</t>
+  </si>
+  <si>
+    <t>Auto Cycle</t>
+  </si>
+  <si>
+    <t>Blade Change</t>
+  </si>
+  <si>
+    <t>Have been removed as LED Indicators at Top of HMI</t>
   </si>
 </sst>
 </file>
@@ -4130,7 +4145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19F8442-ABAB-4CD0-8AEC-54A0D290E2EE}">
   <dimension ref="A1:L451"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -9197,14 +9212,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1173B4E1-7A21-4D96-8FF7-8348F1EA7663}">
-  <dimension ref="A1"/>
+  <dimension ref="A22:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>931</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -9229,8 +9270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95FFEFC-764C-46B6-BD5F-BE7FD7ECF22E}">
   <dimension ref="B2:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="P118" sqref="P118"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Delta RMC200 manuals PDF
</commit_message>
<xml_diff>
--- a/TagListHmi.xlsx
+++ b/TagListHmi.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\J1405-Haynes-SavageSaw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49C27DD-2235-4483-A0A2-32CDC307B136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E002B7C-A44A-41C4-8800-8282A88AFD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6A31735C-1E10-47DA-9BDD-C0801E160811}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6A31735C-1E10-47DA-9BDD-C0801E160811}"/>
   </bookViews>
   <sheets>
     <sheet name="TagListHmi" sheetId="1" r:id="rId1"/>
     <sheet name="Message Library" sheetId="2" r:id="rId2"/>
-    <sheet name="Fault List" sheetId="3" r:id="rId3"/>
-    <sheet name="HMI Screen Shots" sheetId="4" r:id="rId4"/>
+    <sheet name="NotesForSeptVisit" sheetId="5" r:id="rId3"/>
+    <sheet name="Fault List" sheetId="3" r:id="rId4"/>
+    <sheet name="HMI Screen Shots" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="971">
   <si>
     <t>// Name</t>
   </si>
@@ -2937,6 +2938,18 @@
   </si>
   <si>
     <t>Spindle Case Line Blocked</t>
+  </si>
+  <si>
+    <t>Dual or single Solenoid for Clamp and Grippers</t>
+  </si>
+  <si>
+    <t>add estop button</t>
+  </si>
+  <si>
+    <t>Wire #s for home and overtravel switches</t>
+  </si>
+  <si>
+    <t>does the diameter sensor work?  Demonstrate</t>
   </si>
 </sst>
 </file>
@@ -9339,7 +9352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1173B4E1-7A21-4D96-8FF7-8348F1EA7663}">
   <dimension ref="A5:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="R39" sqref="R39:U39"/>
     </sheetView>
   </sheetViews>
@@ -9671,6 +9684,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00052D4-C8E7-41D0-AE01-4D76E44C3A89}">
+  <dimension ref="B5:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>970</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77DFA352-13D8-470E-87A8-3A5B9CC85E55}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -9685,7 +9733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95FFEFC-764C-46B6-BD5F-BE7FD7ECF22E}">
   <dimension ref="B2:O41"/>
   <sheetViews>

</xml_diff>

<commit_message>
added OT Inputs to HMI
</commit_message>
<xml_diff>
--- a/TagListHmi.xlsx
+++ b/TagListHmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\J1405-Haynes-SavageSaw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E002B7C-A44A-41C4-8800-8282A88AFD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5619F0A2-1C18-45D1-A171-8893CDEE1F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6A31735C-1E10-47DA-9BDD-C0801E160811}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="980">
   <si>
     <t>// Name</t>
   </si>
@@ -2950,6 +2950,33 @@
   </si>
   <si>
     <t>does the diameter sensor work?  Demonstrate</t>
+  </si>
+  <si>
+    <t>What is the condition of the cables?  Still fexible?  Oil resistant needed?</t>
+  </si>
+  <si>
+    <t>Where are the encoders located?</t>
+  </si>
+  <si>
+    <t>Will we need a stand for the main enclosure?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bolt to Floor?</t>
+  </si>
+  <si>
+    <t>Review E-Stop  button V</t>
+  </si>
+  <si>
+    <t>How are the wire run to the OT switches?  Conduit? Cable? Individual wires?</t>
+  </si>
+  <si>
+    <t>Switch and Solenoids go from AC to  DC</t>
+  </si>
+  <si>
+    <t>Review machine layout</t>
+  </si>
+  <si>
+    <t>reviewwire colors andterminations</t>
   </si>
 </sst>
 </file>
@@ -9685,10 +9712,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00052D4-C8E7-41D0-AE01-4D76E44C3A89}">
-  <dimension ref="B5:B10"/>
+  <dimension ref="B5:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9703,14 +9730,59 @@
         <v>968</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>969</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>970</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HMI Saw RUN Updated
</commit_message>
<xml_diff>
--- a/TagListHmi.xlsx
+++ b/TagListHmi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\J1405-Haynes-SavageSaw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F149EC-AA09-4EA1-A621-04784741D4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27E33BF-1523-48A7-809E-6CE95CF03D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6A31735C-1E10-47DA-9BDD-C0801E160811}"/>
+    <workbookView xWindow="4035" yWindow="0" windowWidth="21600" windowHeight="15585" activeTab="5" xr2:uid="{6A31735C-1E10-47DA-9BDD-C0801E160811}"/>
   </bookViews>
   <sheets>
     <sheet name="TagListHmi" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="NotesForSeptVisit" sheetId="5" r:id="rId3"/>
     <sheet name="Fault List" sheetId="3" r:id="rId4"/>
     <sheet name="HMI Screen Shots" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="1015">
   <si>
     <t>// Name</t>
   </si>
@@ -2989,6 +2990,99 @@
   </si>
   <si>
     <t>Take L4Computer</t>
+  </si>
+  <si>
+    <t>Control Power On</t>
+  </si>
+  <si>
+    <t>Loop Pump Aux</t>
+  </si>
+  <si>
+    <t>Pump Motor Aux</t>
+  </si>
+  <si>
+    <t>Cooling Fan Aux</t>
+  </si>
+  <si>
+    <t>Swarf Pump Aux</t>
+  </si>
+  <si>
+    <t>Swarf Conveyor Aux</t>
+  </si>
+  <si>
+    <t>Gauge Home Limit</t>
+  </si>
+  <si>
+    <t>Traverse Home Limit</t>
+  </si>
+  <si>
+    <t>Raise Lower Home Limit</t>
+  </si>
+  <si>
+    <t>Guage In OverTravel</t>
+  </si>
+  <si>
+    <t>Gauge Out Overtravel</t>
+  </si>
+  <si>
+    <t>Traverse Forward Overtravel</t>
+  </si>
+  <si>
+    <t>Traverse Reverse Overtravel</t>
+  </si>
+  <si>
+    <t>RaiseOvertravel</t>
+  </si>
+  <si>
+    <t>LowerOvertravel</t>
+  </si>
+  <si>
+    <t>HPU Motor Starter</t>
+  </si>
+  <si>
+    <t>Loop Motor Starter</t>
+  </si>
+  <si>
+    <t>Swarf Motor Starter</t>
+  </si>
+  <si>
+    <t>Swarf Conveyor Starter</t>
+  </si>
+  <si>
+    <t>Laser Line CR</t>
+  </si>
+  <si>
+    <t>Lt Auto On Green</t>
+  </si>
+  <si>
+    <t>Lt Power On Amber</t>
+  </si>
+  <si>
+    <t>Lt Red Axis Active</t>
+  </si>
+  <si>
+    <t>OLD</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Blade Guard</t>
+  </si>
+  <si>
+    <t>Blade Detect</t>
+  </si>
+  <si>
+    <t>Swarf Filter</t>
+  </si>
+  <si>
+    <t>Hyd Cooling</t>
+  </si>
+  <si>
+    <t>Coolant Starter</t>
   </si>
 </sst>
 </file>
@@ -9726,8 +9820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00052D4-C8E7-41D0-AE01-4D76E44C3A89}">
   <dimension ref="B5:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9841,7 +9935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95FFEFC-764C-46B6-BD5F-BE7FD7ECF22E}">
   <dimension ref="B2:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -9864,4 +9958,568 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62625DAA-B9DF-4183-A60B-331047600C88}">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>502</v>
+      </c>
+      <c r="B3">
+        <v>600</v>
+      </c>
+      <c r="C3" t="s">
+        <v>984</v>
+      </c>
+      <c r="F3">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>503</v>
+      </c>
+      <c r="B4">
+        <v>601</v>
+      </c>
+      <c r="C4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F4">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>504</v>
+      </c>
+      <c r="B5">
+        <v>602</v>
+      </c>
+      <c r="C5" t="s">
+        <v>985</v>
+      </c>
+      <c r="F5">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>505</v>
+      </c>
+      <c r="B6">
+        <v>603</v>
+      </c>
+      <c r="C6" t="s">
+        <v>987</v>
+      </c>
+      <c r="F6">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>604</v>
+      </c>
+      <c r="F7">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>534</v>
+      </c>
+      <c r="B8">
+        <v>605</v>
+      </c>
+      <c r="C8" t="s">
+        <v>988</v>
+      </c>
+      <c r="F8">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>535</v>
+      </c>
+      <c r="B9">
+        <v>606</v>
+      </c>
+      <c r="C9" t="s">
+        <v>989</v>
+      </c>
+      <c r="F9">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>607</v>
+      </c>
+      <c r="E10">
+        <v>614</v>
+      </c>
+      <c r="F10">
+        <v>632</v>
+      </c>
+      <c r="G10" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>608</v>
+      </c>
+      <c r="E11">
+        <v>615</v>
+      </c>
+      <c r="F11">
+        <v>633</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>609</v>
+      </c>
+      <c r="E12">
+        <v>616</v>
+      </c>
+      <c r="F12">
+        <v>634</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>610</v>
+      </c>
+      <c r="E13">
+        <v>617</v>
+      </c>
+      <c r="F13">
+        <v>635</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>545</v>
+      </c>
+      <c r="B14">
+        <v>611</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E14">
+        <v>630</v>
+      </c>
+      <c r="F14">
+        <v>636</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>602</v>
+      </c>
+      <c r="B15">
+        <v>612</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E15">
+        <v>631</v>
+      </c>
+      <c r="F15">
+        <v>637</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>603</v>
+      </c>
+      <c r="B16">
+        <v>613</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F16">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>614</v>
+      </c>
+      <c r="F17">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>615</v>
+      </c>
+      <c r="F18">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>516</v>
+      </c>
+      <c r="B19">
+        <v>616</v>
+      </c>
+      <c r="C19" t="s">
+        <v>990</v>
+      </c>
+      <c r="F19">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>517</v>
+      </c>
+      <c r="B20">
+        <v>617</v>
+      </c>
+      <c r="C20" t="s">
+        <v>991</v>
+      </c>
+      <c r="E20">
+        <v>642</v>
+      </c>
+      <c r="F20">
+        <v>642</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>530</v>
+      </c>
+      <c r="B21">
+        <v>618</v>
+      </c>
+      <c r="C21" t="s">
+        <v>992</v>
+      </c>
+      <c r="E21">
+        <v>643</v>
+      </c>
+      <c r="F21">
+        <v>643</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>531</v>
+      </c>
+      <c r="B22">
+        <v>619</v>
+      </c>
+      <c r="C22" t="s">
+        <v>993</v>
+      </c>
+      <c r="E22">
+        <v>644</v>
+      </c>
+      <c r="F22">
+        <v>644</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>532</v>
+      </c>
+      <c r="B23">
+        <v>620</v>
+      </c>
+      <c r="C23" t="s">
+        <v>994</v>
+      </c>
+      <c r="E23">
+        <v>645</v>
+      </c>
+      <c r="F23">
+        <v>645</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>533</v>
+      </c>
+      <c r="B24">
+        <v>621</v>
+      </c>
+      <c r="C24" t="s">
+        <v>995</v>
+      </c>
+      <c r="F24">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>542</v>
+      </c>
+      <c r="B25">
+        <v>622</v>
+      </c>
+      <c r="C25" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>543</v>
+      </c>
+      <c r="B26">
+        <v>623</v>
+      </c>
+      <c r="C26" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>544</v>
+      </c>
+      <c r="B27">
+        <v>624</v>
+      </c>
+      <c r="C27" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>614</v>
+      </c>
+      <c r="B35">
+        <v>632</v>
+      </c>
+      <c r="C35" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>615</v>
+      </c>
+      <c r="B36">
+        <v>633</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>616</v>
+      </c>
+      <c r="B37">
+        <v>634</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>617</v>
+      </c>
+      <c r="B38">
+        <v>635</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>630</v>
+      </c>
+      <c r="B39">
+        <v>636</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>631</v>
+      </c>
+      <c r="B40">
+        <v>637</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>642</v>
+      </c>
+      <c r="B45">
+        <v>642</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>643</v>
+      </c>
+      <c r="B46">
+        <v>643</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>644</v>
+      </c>
+      <c r="B47">
+        <v>644</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>645</v>
+      </c>
+      <c r="B48">
+        <v>645</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>646</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>